<commit_message>
assigned login scenarios completed
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -26,7 +26,7 @@
     <t>errorMessage</t>
   </si>
   <si>
-    <t>invalid credentials</t>
+    <t>invalid_credentials</t>
   </si>
   <si>
     <t>invalid</t>
@@ -35,22 +35,22 @@
     <t>Invalid username and password Please try again</t>
   </si>
   <si>
-    <t>empty username</t>
+    <t>empty_username</t>
+  </si>
+  <si>
+    <t>March@2025</t>
+  </si>
+  <si>
+    <t>Please enter your user name</t>
+  </si>
+  <si>
+    <t>empty_password</t>
   </si>
   <si>
     <t>Playwright@gmail.com</t>
   </si>
   <si>
-    <t>wrongpass</t>
-  </si>
-  <si>
-    <t>empty password</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>March@2025</t>
+    <t>Please enter your password</t>
   </si>
 </sst>
 </file>
@@ -312,6 +312,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.5"/>
+    <col customWidth="1" min="2" max="2" width="18.0"/>
+    <col customWidth="1" min="4" max="4" width="36.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -346,10 +348,10 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -360,7 +362,7 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Batch DDT Added Succesfully
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="class" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="batch" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="class" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>scenario</t>
   </si>
@@ -26,7 +27,7 @@
     <t>errorMessage</t>
   </si>
   <si>
-    <t>invalid credentials</t>
+    <t>invalid_credentials</t>
   </si>
   <si>
     <t>invalid</t>
@@ -35,29 +36,53 @@
     <t>Invalid username and password Please try again</t>
   </si>
   <si>
-    <t>empty username</t>
+    <t>empty_username</t>
+  </si>
+  <si>
+    <t>March@2025</t>
+  </si>
+  <si>
+    <t>Please enter your user name</t>
+  </si>
+  <si>
+    <t>empty_password</t>
   </si>
   <si>
     <t>Playwright@gmail.com</t>
   </si>
   <si>
-    <t>wrongpass</t>
-  </si>
-  <si>
-    <t>empty password</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>March@2025</t>
+    <t>Please enter your password</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
+    <t>BatchName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>NumberOfClasses</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>PleaseDontDelete</t>
+  </si>
+  <si>
+    <t>Anu</t>
+  </si>
+  <si>
+    <t>Successss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -68,6 +93,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,12 +113,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -104,6 +142,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -312,6 +354,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.5"/>
+    <col customWidth="1" min="2" max="2" width="18.0"/>
+    <col customWidth="1" min="4" max="4" width="36.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -346,10 +390,10 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -360,7 +404,7 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -370,6 +414,61 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="14.38"/>
+    <col customWidth="1" min="3" max="3" width="9.75"/>
+    <col customWidth="1" min="4" max="4" width="9.38"/>
+    <col customWidth="1" min="5" max="5" width="15.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4">
+        <v>12.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Fix file path separators in feature tests and update .gitignore for test data
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -4,8 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="batch" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="class" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="program" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="batch" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="class" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>scenario</t>
   </si>
@@ -57,25 +58,31 @@
     <t>ProgramName</t>
   </si>
   <si>
-    <t>BatchName</t>
+    <t>Description</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>PName</t>
+  </si>
+  <si>
+    <t>PnameDes</t>
+  </si>
+  <si>
+    <t>BatchName</t>
   </si>
   <si>
     <t>NumberOfClasses</t>
   </si>
   <si>
-    <t>valid</t>
-  </si>
-  <si>
     <t>PleaseDontDelete</t>
   </si>
   <si>
-    <t>Rixx</t>
+    <t>Son</t>
   </si>
   <si>
-    <t>Reo</t>
+    <t>Sec</t>
   </si>
   <si>
     <t>batchName</t>
@@ -215,6 +222,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -491,6 +502,43 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="14.38"/>
     <col customWidth="1" min="3" max="3" width="9.75"/>
@@ -506,27 +554,27 @@
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4">
         <v>25.0</v>
@@ -537,7 +585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -560,28 +608,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -603,31 +651,31 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -649,20 +697,20 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8">
         <v>45747.0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>

</xml_diff>

<commit_message>
add new class completed
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -4,8 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="batch" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="class" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="program" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="batch" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="class" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>scenario</t>
   </si>
@@ -57,25 +58,31 @@
     <t>ProgramName</t>
   </si>
   <si>
-    <t>BatchName</t>
+    <t>Description</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>PName</t>
+  </si>
+  <si>
+    <t>PnameDes</t>
+  </si>
+  <si>
+    <t>BatchName</t>
   </si>
   <si>
     <t>NumberOfClasses</t>
   </si>
   <si>
-    <t>valid</t>
-  </si>
-  <si>
     <t>PleaseDontDelete</t>
   </si>
   <si>
-    <t>Rixx</t>
+    <t>Son</t>
   </si>
   <si>
-    <t>Reo</t>
+    <t>Sec</t>
   </si>
   <si>
     <t>batchName</t>
@@ -130,6 +137,30 @@
   </si>
   <si>
     <t>onlyMandatory</t>
+  </si>
+  <si>
+    <t>onlyOptional</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>added comments</t>
+  </si>
+  <si>
+    <t>added notes</t>
+  </si>
+  <si>
+    <t>uploaded recording</t>
+  </si>
+  <si>
+    <t>invalidData</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>invalid!!!!</t>
   </si>
 </sst>
 </file>
@@ -215,6 +246,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -491,6 +526,43 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="14.38"/>
     <col customWidth="1" min="3" max="3" width="9.75"/>
@@ -506,27 +578,27 @@
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4">
         <v>25.0</v>
@@ -537,7 +609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -560,28 +632,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -603,31 +675,31 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -649,20 +721,20 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8">
         <v>45747.0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -686,14 +758,25 @@
       <c r="Z3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="G4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -713,15 +796,29 @@
       <c r="Z4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="C5" s="5">
+        <v>1234.0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1234.0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="G5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>

</xml_diff>

<commit_message>
Enable fully parallel test execution and update program search functionality
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -624,50 +624,56 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1">
-        <v>25.0</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1">
-        <v>1111.0</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
-        <v>2.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="1">
+        <v>1111.0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
         <v>2018.0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <v>11.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add validation scenarios for program name input in Admin module
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>scenario</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t>PnameDes</t>
+  </si>
+  <si>
+    <t>invalidPName</t>
+  </si>
+  <si>
+    <t>PName123</t>
+  </si>
+  <si>
+    <t>specialChar</t>
+  </si>
+  <si>
+    <t>PN@#$</t>
+  </si>
+  <si>
+    <t>min2Char</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>cd</t>
   </si>
   <si>
     <t>BatchName</t>
@@ -130,7 +151,7 @@
     <t>Java Batch 01</t>
   </si>
   <si>
-    <t>playwrightWizardJava</t>
+    <t>playwrightWizard</t>
   </si>
   <si>
     <t>desc</t>
@@ -154,7 +175,7 @@
     <t>onlyMandatory</t>
   </si>
   <si>
-    <t>playwrightWizardSelenium</t>
+    <t>playwrightWizardS</t>
   </si>
   <si>
     <t>onlyOptional</t>
@@ -567,6 +588,39 @@
         <v>17</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -597,13 +651,13 @@
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -611,13 +665,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4">
         <v>9.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E2" s="4">
         <v>25.0</v>
@@ -631,13 +685,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1">
         <v>25.0</v>
@@ -645,16 +699,16 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>1111.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1">
         <v>2.0</v>
@@ -662,16 +716,16 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1">
         <v>2018.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1">
         <v>11.0</v>
@@ -705,28 +759,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -748,31 +802,31 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -794,20 +848,20 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8">
         <v>45747.0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -832,23 +886,23 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -870,7 +924,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5">
@@ -880,17 +934,17 @@
         <v>1234.0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>

</xml_diff>

<commit_message>
Add validation for program name and description in Admin module
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>scenario</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>cd</t>
+  </si>
+  <si>
+    <t>emptyDes</t>
   </si>
   <si>
     <t>BatchName</t>
@@ -621,6 +624,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -651,13 +662,13 @@
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -665,13 +676,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4">
         <v>9.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" s="4">
         <v>25.0</v>
@@ -685,13 +696,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1">
         <v>25.0</v>
@@ -699,16 +710,16 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1">
         <v>1111.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1">
         <v>2.0</v>
@@ -716,16 +727,16 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1">
         <v>2018.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1">
         <v>11.0</v>
@@ -759,28 +770,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -802,31 +813,31 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -848,20 +859,20 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8">
         <v>45747.0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -886,23 +897,23 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -924,7 +935,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5">
@@ -934,17 +945,17 @@
         <v>1234.0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>

</xml_diff>

<commit_message>
sorting completed in class
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -130,7 +130,7 @@
     <t>Java Batch 01</t>
   </si>
   <si>
-    <t>playwrightWizardJava</t>
+    <t>playwrightWizard</t>
   </si>
   <si>
     <t>desc</t>
@@ -154,7 +154,7 @@
     <t>onlyMandatory</t>
   </si>
   <si>
-    <t>playwrightWizardSelenium</t>
+    <t>playwrightWizardS</t>
   </si>
   <si>
     <t>onlyOptional</t>
@@ -624,50 +624,56 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1">
-        <v>25.0</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1">
-        <v>1111.0</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
-        <v>2.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="1">
+        <v>1111.0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
         <v>2018.0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <v>11.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit Batch and Sort Batch Completed
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>scenario</t>
   </si>
@@ -106,28 +106,37 @@
     <t>NumberOfClasses</t>
   </si>
   <si>
-    <t>PNameANR</t>
+    <t>AnuBatch</t>
   </si>
   <si>
-    <t>Sec</t>
+    <t>Anusuya</t>
   </si>
   <si>
     <t>missingmandatory</t>
   </si>
   <si>
-    <t>drf</t>
-  </si>
-  <si>
     <t>validmandatesave</t>
-  </si>
-  <si>
-    <t>juju</t>
   </si>
   <si>
     <t>cancel</t>
   </si>
   <si>
-    <t>hhh</t>
+    <t>editvaliddata</t>
+  </si>
+  <si>
+    <t>Vinod</t>
+  </si>
+  <si>
+    <t>editinvaliddata</t>
+  </si>
+  <si>
+    <t>%%^</t>
+  </si>
+  <si>
+    <t>editvaliddatacancel</t>
+  </si>
+  <si>
+    <t>Arnik</t>
   </si>
   <si>
     <t>batchName</t>
@@ -209,6 +218,33 @@
   </si>
   <si>
     <t>invalid!!!!</t>
+  </si>
+  <si>
+    <t>editAll</t>
+  </si>
+  <si>
+    <t>updated desc</t>
+  </si>
+  <si>
+    <t>arunasel S</t>
+  </si>
+  <si>
+    <t>updated comments</t>
+  </si>
+  <si>
+    <t>updated notes</t>
+  </si>
+  <si>
+    <t>updated recording</t>
+  </si>
+  <si>
+    <t>editMandatory</t>
+  </si>
+  <si>
+    <t>editInvalidData</t>
+  </si>
+  <si>
+    <t>editOptional</t>
   </si>
 </sst>
 </file>
@@ -664,7 +700,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.5"/>
+    <col customWidth="1" min="1" max="1" width="18.5"/>
     <col customWidth="1" min="2" max="2" width="14.38"/>
     <col customWidth="1" min="3" max="3" width="9.75"/>
     <col customWidth="1" min="4" max="4" width="9.38"/>
@@ -696,7 +732,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="4">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>31</v>
@@ -706,10 +742,21 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1">
+        <v>98.0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1">
+        <v>222.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -719,44 +766,77 @@
         <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1">
-        <v>25.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1">
-        <v>1111.0</v>
+        <v>23.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1">
-        <v>2.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="1">
-        <v>2018.0</v>
+        <v>88.0</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1">
+        <v>299.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="1">
-        <v>11.0</v>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3.42434434E8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1">
+        <v>904.0</v>
       </c>
     </row>
   </sheetData>
@@ -787,28 +867,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -830,31 +910,31 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -876,20 +956,20 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8">
         <v>45747.0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -914,23 +994,23 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -952,7 +1032,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5">
@@ -962,17 +1042,17 @@
         <v>1234.0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -993,15 +1073,29 @@
       <c r="Z5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="D6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="8">
+        <v>45747.0</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -1021,12 +1115,18 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="7"/>
+      <c r="A7" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1049,15 +1149,27 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="7"/>
+      <c r="A8" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="5">
+        <v>1234.0</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="G8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -1077,15 +1189,23 @@
       <c r="Z8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="G9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>

</xml_diff>

<commit_message>
Add program name for chaining and enhance delete feature scenarios
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
   <si>
     <t>scenario</t>
   </si>
@@ -100,6 +100,12 @@
     <t>editDes</t>
   </si>
   <si>
+    <t>valid for chaining</t>
+  </si>
+  <si>
+    <t>Desforchaining</t>
+  </si>
+  <si>
     <t>BatchName</t>
   </si>
   <si>
@@ -110,6 +116,9 @@
   </si>
   <si>
     <t>Anusuya</t>
+  </si>
+  <si>
+    <t>mandatory</t>
   </si>
   <si>
     <t>missingmandatory</t>
@@ -685,6 +694,17 @@
         <v>27</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -715,13 +735,13 @@
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -729,13 +749,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4">
-        <v>45.0</v>
+        <v>334.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4">
         <v>25.0</v>
@@ -743,16 +763,16 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1">
-        <v>29.0</v>
+        <v>234.0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1">
         <v>222.0</v>
@@ -760,13 +780,13 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1">
         <v>22.0</v>
@@ -774,16 +794,16 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1">
-        <v>22.0</v>
+        <v>222.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1">
         <v>32.0</v>
@@ -791,16 +811,16 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>22.0</v>
+        <v>890.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1">
         <v>33.0</v>
@@ -808,10 +828,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1">
         <v>299.0</v>
@@ -819,10 +839,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1">
         <v>3.42434434E8</v>
@@ -830,10 +850,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1">
         <v>904.0</v>
@@ -867,28 +887,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -910,31 +930,31 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -956,20 +976,20 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8">
         <v>45747.0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -994,23 +1014,23 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -1032,7 +1052,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5">
@@ -1042,17 +1062,17 @@
         <v>1234.0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -1074,27 +1094,27 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E6" s="8">
         <v>45747.0</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -1116,16 +1136,16 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1150,7 +1170,7 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1158,17 +1178,17 @@
         <v>1234.0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1190,7 +1210,7 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1198,13 +1218,13 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>

</xml_diff>

<commit_message>
Added changes to logout
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t>scenario</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Anusuya</t>
+  </si>
+  <si>
+    <t>mandatory</t>
   </si>
   <si>
     <t>missingmandatory</t>
@@ -732,7 +735,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="4">
-        <v>45.0</v>
+        <v>334.0</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>31</v>
@@ -743,13 +746,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="1">
-        <v>29.0</v>
+        <v>234.0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -760,7 +763,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>30</v>
@@ -774,13 +777,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1">
-        <v>22.0</v>
+        <v>222.0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>31</v>
@@ -791,13 +794,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="1">
-        <v>22.0</v>
+        <v>890.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>31</v>
@@ -808,10 +811,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1">
         <v>299.0</v>
@@ -819,10 +822,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1">
         <v>3.42434434E8</v>
@@ -830,10 +833,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1">
         <v>904.0</v>
@@ -867,28 +870,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -910,31 +913,31 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -956,20 +959,20 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8">
         <v>45747.0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -994,23 +997,23 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -1032,7 +1035,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5">
@@ -1042,17 +1045,17 @@
         <v>1234.0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -1074,27 +1077,27 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E6" s="8">
         <v>45747.0</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -1116,16 +1119,16 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1150,7 +1153,7 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1158,17 +1161,17 @@
         <v>1234.0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1190,7 +1193,7 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1198,13 +1201,13 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>

</xml_diff>

<commit_message>
Full process chaining completed
</commit_message>
<xml_diff>
--- a/tests/testData.xlsx
+++ b/tests/testData.xlsx
@@ -625,6 +625,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="19.25"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -758,13 +761,13 @@
         <v>32</v>
       </c>
       <c r="C2" s="4">
-        <v>72.0</v>
+        <v>101.0</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="4">
-        <v>25.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="3">
@@ -775,13 +778,13 @@
         <v>32</v>
       </c>
       <c r="C3" s="1">
-        <v>81.0</v>
+        <v>201.0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="1">
-        <v>222.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="4">
@@ -806,7 +809,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="1">
-        <v>218.0</v>
+        <v>301.0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>33</v>
@@ -823,7 +826,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>616.0</v>
+        <v>401.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>33</v>

</xml_diff>